<commit_message>
updated the planning and expanded the callback example
</commit_message>
<xml_diff>
--- a/Planning/Planning Mart-Jan.xlsx
+++ b/Planning/Planning Mart-Jan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmeer\Crownstone\Crownstone-Intern-Files\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1866602E-4253-476F-8447-0A854B9BDCD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE26B74-492B-4EE0-8FB7-0448922A6D53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{435FE1F0-6994-48E1-B549-92D4C1B2F0F0}"/>
   </bookViews>
@@ -1029,7 +1029,7 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1135,7 @@
       <c r="E2" s="2">
         <v>44095</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="2">
         <v>44102</v>
       </c>
       <c r="G2" s="8">
@@ -1757,6 +1757,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3B7FDB071B5114F9C1E9BE4F6100C6D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd5f6a8e33fa3fa4a319a3581ac19cf9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3c4e9300-2158-4f27-b7a4-0ea661d6437f" xmlns:ns4="72caab85-b177-4a5e-b33a-cb569996d4d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e863128cda4ce81bacfd61d68ec5d105" ns3:_="" ns4:_="">
     <xsd:import namespace="3c4e9300-2158-4f27-b7a4-0ea661d6437f"/>
@@ -1979,22 +1994,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07E1F462-3555-42C8-855E-56779F9BD1EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C82C6B7-F5A9-4C61-A0FE-73C6A14DE687}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C14C440-8045-4B84-ADF1-362E77187BD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2011,21 +2028,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C82C6B7-F5A9-4C61-A0FE-73C6A14DE687}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07E1F462-3555-42C8-855E-56779F9BD1EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
made a new component diagram
</commit_message>
<xml_diff>
--- a/Planning/Planning Mart-Jan.xlsx
+++ b/Planning/Planning Mart-Jan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmeer\Crownstone\Crownstone-Intern-Files\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE26B74-492B-4EE0-8FB7-0448922A6D53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B9C845-7849-400E-BCFD-604301AF4B5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{435FE1F0-6994-48E1-B549-92D4C1B2F0F0}"/>
+    <workbookView xWindow="5250" yWindow="3180" windowWidth="21600" windowHeight="11385" xr2:uid="{435FE1F0-6994-48E1-B549-92D4C1B2F0F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1029,17 +1029,18 @@
   <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.28515625" customWidth="1"/>
@@ -1138,7 +1139,7 @@
       <c r="F2" s="2">
         <v>44102</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="2">
         <v>44109</v>
       </c>
       <c r="H2" s="8">
@@ -1211,7 +1212,7 @@
       <c r="E3" s="3">
         <v>44096</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="3">
         <v>44103</v>
       </c>
       <c r="G3" s="6">
@@ -1287,7 +1288,7 @@
       <c r="E4" s="3">
         <v>44097</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="3">
         <v>44104</v>
       </c>
       <c r="G4" s="6">
@@ -1363,7 +1364,7 @@
       <c r="E5" s="3">
         <v>44098</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="3">
         <v>44105</v>
       </c>
       <c r="G5" s="6">
@@ -1439,7 +1440,7 @@
       <c r="E6" s="5">
         <v>44099</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="5">
         <v>44106</v>
       </c>
       <c r="G6" s="7">
@@ -1547,17 +1548,17 @@
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="23"/>
+      <c r="G8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="23"/>
+      <c r="L8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="L8" s="23"/>
       <c r="M8" s="23"/>
       <c r="N8" s="23"/>
       <c r="O8" s="23"/>
@@ -1596,14 +1597,14 @@
       <c r="D9" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="H9" s="13" t="s">
         <v>42</v>
@@ -1757,21 +1758,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3B7FDB071B5114F9C1E9BE4F6100C6D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd5f6a8e33fa3fa4a319a3581ac19cf9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3c4e9300-2158-4f27-b7a4-0ea661d6437f" xmlns:ns4="72caab85-b177-4a5e-b33a-cb569996d4d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e863128cda4ce81bacfd61d68ec5d105" ns3:_="" ns4:_="">
     <xsd:import namespace="3c4e9300-2158-4f27-b7a4-0ea661d6437f"/>
@@ -1994,24 +1980,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07E1F462-3555-42C8-855E-56779F9BD1EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C82C6B7-F5A9-4C61-A0FE-73C6A14DE687}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C14C440-8045-4B84-ADF1-362E77187BD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2028,4 +2012,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C82C6B7-F5A9-4C61-A0FE-73C6A14DE687}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07E1F462-3555-42C8-855E-56779F9BD1EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated planning, added vacation days
</commit_message>
<xml_diff>
--- a/Planning/Planning Mart-Jan.xlsx
+++ b/Planning/Planning Mart-Jan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmeer\Crownstone\Crownstone-Intern-Files\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D77C24E-B4A6-4D2C-8E96-7B7B201FEA01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A443BC92-2CEE-4730-8818-2943108F2E03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5175" yWindow="3135" windowWidth="21600" windowHeight="11385" xr2:uid="{435FE1F0-6994-48E1-B549-92D4C1B2F0F0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{435FE1F0-6994-48E1-B549-92D4C1B2F0F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>Gesprek docent</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t>No workday</t>
+  </si>
+  <si>
+    <t>Vacationday</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -573,6 +576,8 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1020,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBB7574-35C6-452D-81F0-06F94FE9DD1B}">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1033,8 +1038,9 @@
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
     <col min="5" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="21" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.28515625" customWidth="1"/>
@@ -1136,7 +1142,7 @@
       <c r="G2" s="2">
         <v>44109</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="2">
         <v>44116</v>
       </c>
       <c r="I2" s="8">
@@ -1291,7 +1297,7 @@
       <c r="H4" s="6">
         <v>44118</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="43">
         <v>44125</v>
       </c>
       <c r="J4" s="6">
@@ -1367,7 +1373,7 @@
       <c r="H5" s="6">
         <v>44119</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="43">
         <v>44126</v>
       </c>
       <c r="J5" s="6">
@@ -1437,7 +1443,7 @@
       <c r="F6" s="5">
         <v>44106</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <v>44113</v>
       </c>
       <c r="H6" s="7">
@@ -1597,11 +1603,11 @@
       <c r="F9" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="12" t="s">
         <v>43</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>42</v>
@@ -1739,6 +1745,11 @@
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1752,21 +1763,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3B7FDB071B5114F9C1E9BE4F6100C6D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fd5f6a8e33fa3fa4a319a3581ac19cf9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3c4e9300-2158-4f27-b7a4-0ea661d6437f" xmlns:ns4="72caab85-b177-4a5e-b33a-cb569996d4d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e863128cda4ce81bacfd61d68ec5d105" ns3:_="" ns4:_="">
     <xsd:import namespace="3c4e9300-2158-4f27-b7a4-0ea661d6437f"/>
@@ -1989,24 +1985,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07E1F462-3555-42C8-855E-56779F9BD1EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C82C6B7-F5A9-4C61-A0FE-73C6A14DE687}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C14C440-8045-4B84-ADF1-362E77187BD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2023,4 +2017,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C82C6B7-F5A9-4C61-A0FE-73C6A14DE687}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07E1F462-3555-42C8-855E-56779F9BD1EF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated planning and updated planning diagram
</commit_message>
<xml_diff>
--- a/Planning/Planning Mart-Jan.xlsx
+++ b/Planning/Planning Mart-Jan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmeer\Crownstone\Crownstone-Intern-Files\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B95A03-0EDA-456D-9550-2FBE8A01FA72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC1EA89-07E0-4533-8533-4DC5E1FF78D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{435FE1F0-6994-48E1-B549-92D4C1B2F0F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="64">
   <si>
     <t>1</t>
   </si>
@@ -216,6 +216,15 @@
   </si>
   <si>
     <t>Phase 3 - Extension week</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
   </si>
 </sst>
 </file>
@@ -527,9 +536,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -541,7 +549,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -552,7 +559,6 @@
     <xf numFmtId="165" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -586,11 +592,28 @@
     <xf numFmtId="165" fontId="0" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="17" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="28">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
@@ -704,33 +727,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3791D96-3CE9-4F8A-BC26-EFEC56076E33}" name="Table1" displayName="Table1" ref="A1:X10" totalsRowShown="0" headerRowDxfId="24" tableBorderDxfId="23">
-  <autoFilter ref="A1:X10" xr:uid="{110C82E6-A843-4040-A019-B1924DCB1DD2}"/>
-  <tableColumns count="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3791D96-3CE9-4F8A-BC26-EFEC56076E33}" name="Table1" displayName="Table1" ref="A1:AA10" totalsRowShown="0" headerRowDxfId="27" tableBorderDxfId="26">
+  <autoFilter ref="A1:AA10" xr:uid="{110C82E6-A843-4040-A019-B1924DCB1DD2}"/>
+  <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{D3A09CF0-3BAF-407A-B529-43EDDD215D27}" name="Weeks"/>
-    <tableColumn id="2" xr3:uid="{5490862F-B7D0-4928-BDBE-9E779B30CC2B}" name="1" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{48A2C1F8-24BF-4DCA-9316-7A0BE338A9B4}" name="2" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{9D9879AC-15BD-4532-AE3C-35725E207578}" name="3" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{D2520B3A-7A26-4B15-A44B-34EBDA7C2E97}" name="4" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{25D25D94-43F5-4027-9FB9-EF79C35E4C45}" name="5" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{17F1938F-9D4F-4D45-AC6D-DB3323D37429}" name="6" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{352CC87D-E430-47D7-9139-737EDA50DAB6}" name="7" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{4EF48C1C-3837-4E5A-B970-06BE5F7A4591}" name="8" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{16A53116-19BF-47DA-B5DE-714631567A41}" name="9" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{5E66304B-73E5-44EF-AB13-0C7914CD01B5}" name="10" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{9FACBA77-1401-4C28-ABDF-ED79CCE609FA}" name="11" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{69904905-162B-4F6A-BD7D-D7B55DF37613}" name="12" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{142C7A06-3502-45E1-B592-6E803ACEC2A6}" name="13" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{F2D343CD-29AF-43E2-9B35-D5100ED3B155}" name="14" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{515FF106-3985-4596-BCC0-EE115C856B45}" name="15" dataDxfId="8"/>
-    <tableColumn id="17" xr3:uid="{9E462F55-7B19-46BD-93CA-7EA1205D1FCD}" name="16" dataDxfId="7"/>
-    <tableColumn id="18" xr3:uid="{8FA39420-6302-425E-8CF6-B7C723F93552}" name="17" dataDxfId="6"/>
-    <tableColumn id="19" xr3:uid="{1C2AB089-DF2C-4BDE-825D-F830FE44AF47}" name="18" dataDxfId="5"/>
-    <tableColumn id="20" xr3:uid="{CBA0B86D-EC89-4298-8DBE-4514C82188B4}" name="19" dataDxfId="4"/>
-    <tableColumn id="21" xr3:uid="{A7689F55-DC66-45E7-BD15-71CF51CBEA69}" name="20" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{0411F5E4-1D24-4658-8B38-3F9138BBE94F}" name="21" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{4E2082DC-6BE4-46E7-9818-1FE105940226}" name="22" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{2BF9B189-EE0F-4317-A3B6-0E349E929051}" name="23" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{5490862F-B7D0-4928-BDBE-9E779B30CC2B}" name="1" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{48A2C1F8-24BF-4DCA-9316-7A0BE338A9B4}" name="2" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{9D9879AC-15BD-4532-AE3C-35725E207578}" name="3" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{D2520B3A-7A26-4B15-A44B-34EBDA7C2E97}" name="4" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{25D25D94-43F5-4027-9FB9-EF79C35E4C45}" name="5" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{17F1938F-9D4F-4D45-AC6D-DB3323D37429}" name="6" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{352CC87D-E430-47D7-9139-737EDA50DAB6}" name="7" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{4EF48C1C-3837-4E5A-B970-06BE5F7A4591}" name="8" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{16A53116-19BF-47DA-B5DE-714631567A41}" name="9" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{5E66304B-73E5-44EF-AB13-0C7914CD01B5}" name="10" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{9FACBA77-1401-4C28-ABDF-ED79CCE609FA}" name="11" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{69904905-162B-4F6A-BD7D-D7B55DF37613}" name="12" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{142C7A06-3502-45E1-B592-6E803ACEC2A6}" name="13" dataDxfId="13"/>
+    <tableColumn id="15" xr3:uid="{F2D343CD-29AF-43E2-9B35-D5100ED3B155}" name="14" dataDxfId="12"/>
+    <tableColumn id="16" xr3:uid="{515FF106-3985-4596-BCC0-EE115C856B45}" name="15" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{9E462F55-7B19-46BD-93CA-7EA1205D1FCD}" name="16" dataDxfId="10"/>
+    <tableColumn id="18" xr3:uid="{8FA39420-6302-425E-8CF6-B7C723F93552}" name="17" dataDxfId="9"/>
+    <tableColumn id="19" xr3:uid="{1C2AB089-DF2C-4BDE-825D-F830FE44AF47}" name="18" dataDxfId="8"/>
+    <tableColumn id="20" xr3:uid="{CBA0B86D-EC89-4298-8DBE-4514C82188B4}" name="19" dataDxfId="7"/>
+    <tableColumn id="21" xr3:uid="{A7689F55-DC66-45E7-BD15-71CF51CBEA69}" name="20" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{0411F5E4-1D24-4658-8B38-3F9138BBE94F}" name="21" dataDxfId="5"/>
+    <tableColumn id="23" xr3:uid="{4E2082DC-6BE4-46E7-9818-1FE105940226}" name="22" dataDxfId="4"/>
+    <tableColumn id="24" xr3:uid="{2BF9B189-EE0F-4317-A3B6-0E349E929051}" name="23" dataDxfId="3"/>
+    <tableColumn id="25" xr3:uid="{FC48ADA7-48D0-4A51-A79E-7947E44B3076}" name="24" dataDxfId="2"/>
+    <tableColumn id="26" xr3:uid="{FFD9A8AC-B0E5-4CF2-B9DC-7A69B51AC315}" name="25" dataDxfId="1"/>
+    <tableColumn id="27" xr3:uid="{01E7FD74-FF6E-4CBF-B2C5-30FA21420733}" name="26" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1033,10 +1059,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBB7574-35C6-452D-81F0-06F94FE9DD1B}">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:AA15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,709 +1080,778 @@
     <col min="18" max="20" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="23" max="23" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="S1" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="T1" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="U1" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="V1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="W1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="X1" s="23" t="s">
         <v>38</v>
       </c>
+      <c r="Y1" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="AA1" s="23" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>44074</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>44081</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>44088</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>44095</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>44102</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>44109</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>44116</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>44123</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>44130</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>44137</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>44144</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>44151</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>44158</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>44165</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>44172</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="1">
         <v>44179</v>
       </c>
-      <c r="R2" s="45">
+      <c r="R2" s="42">
         <v>44186</v>
       </c>
-      <c r="S2" s="45">
+      <c r="S2" s="42">
         <v>44193</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
         <v>44200</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="1">
         <v>44207</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="1">
         <v>44214</v>
       </c>
-      <c r="W2" s="8">
+      <c r="W2" s="7">
         <v>44221</v>
       </c>
-      <c r="X2" s="16">
+      <c r="X2" s="14">
         <v>44228</v>
       </c>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
+      <c r="Y2" s="14">
+        <v>44235</v>
+      </c>
+      <c r="Z2" s="45">
+        <v>44242</v>
+      </c>
+      <c r="AA2" s="45">
+        <v>44249</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>44075</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>44082</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>44089</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>44096</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>44103</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>44110</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>44117</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>44124</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <v>44131</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="2">
         <v>44138</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <v>44145</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="2">
         <v>44152</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="2">
         <v>44159</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="2">
         <v>44166</v>
       </c>
-      <c r="P3" s="3">
+      <c r="P3" s="2">
         <v>44173</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="2">
         <v>44180</v>
       </c>
-      <c r="R3" s="43">
+      <c r="R3" s="40">
         <v>44187</v>
       </c>
-      <c r="S3" s="43">
+      <c r="S3" s="40">
         <v>44194</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3" s="2">
         <v>44201</v>
       </c>
-      <c r="U3" s="3">
+      <c r="U3" s="2">
         <v>44208</v>
       </c>
-      <c r="V3" s="3">
+      <c r="V3" s="2">
         <v>44215</v>
       </c>
-      <c r="W3" s="6">
+      <c r="W3" s="5">
         <v>44222</v>
       </c>
-      <c r="X3" s="18">
+      <c r="X3" s="16">
         <v>44229</v>
       </c>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
+      <c r="Y3" s="16">
+        <v>44236</v>
+      </c>
+      <c r="Z3" s="46">
+        <v>44243</v>
+      </c>
+      <c r="AA3" s="46">
+        <v>44250</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>44076</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>44083</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>44090</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>44097</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>44104</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>44111</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>44118</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="40">
         <v>44125</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <v>44132</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>44139</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>44146</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="2">
         <v>44153</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>44160</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <v>44167</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P4" s="2">
         <v>44174</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q4" s="2">
         <v>44181</v>
       </c>
-      <c r="R4" s="43">
+      <c r="R4" s="40">
         <v>44188</v>
       </c>
-      <c r="S4" s="43">
+      <c r="S4" s="40">
         <v>44195</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="2">
         <v>44202</v>
       </c>
-      <c r="U4" s="3">
+      <c r="U4" s="2">
         <v>44209</v>
       </c>
-      <c r="V4" s="3">
+      <c r="V4" s="2">
         <v>44216</v>
       </c>
-      <c r="W4" s="6">
+      <c r="W4" s="5">
         <v>44223</v>
       </c>
-      <c r="X4" s="18">
+      <c r="X4" s="16">
         <v>44230</v>
       </c>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
+      <c r="Y4" s="16">
+        <v>44237</v>
+      </c>
+      <c r="Z4" s="46">
+        <v>44244</v>
+      </c>
+      <c r="AA4" s="46">
+        <v>44251</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>44077</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>44084</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>44091</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>44098</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>44105</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>44112</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>44119</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="40">
         <v>44126</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <v>44133</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>44140</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>44147</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5" s="2">
         <v>44154</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="2">
         <v>44161</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="2">
         <v>44168</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="2">
         <v>44175</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5" s="2">
         <v>44182</v>
       </c>
-      <c r="R5" s="43">
+      <c r="R5" s="40">
         <v>44189</v>
       </c>
-      <c r="S5" s="43">
+      <c r="S5" s="40">
         <v>44196</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5" s="2">
         <v>44203</v>
       </c>
-      <c r="U5" s="3">
+      <c r="U5" s="2">
         <v>44210</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="2">
         <v>44217</v>
       </c>
-      <c r="W5" s="6">
+      <c r="W5" s="5">
         <v>44224</v>
       </c>
-      <c r="X5" s="18">
+      <c r="X5" s="16">
         <v>44231</v>
       </c>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
+      <c r="Y5" s="16">
+        <v>44238</v>
+      </c>
+      <c r="Z5" s="46">
+        <v>44245</v>
+      </c>
+      <c r="AA5" s="46">
+        <v>44252</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>44078</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>44085</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>44092</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>44099</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>44106</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>44113</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>44120</v>
       </c>
-      <c r="I6" s="44">
+      <c r="I6" s="41">
         <v>44127</v>
       </c>
-      <c r="J6" s="44">
+      <c r="J6" s="41">
         <v>44134</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="4">
         <v>44141</v>
       </c>
-      <c r="L6" s="44">
+      <c r="L6" s="41">
         <v>44148</v>
       </c>
-      <c r="M6" s="44">
+      <c r="M6" s="41">
         <v>44155</v>
       </c>
-      <c r="N6" s="44">
+      <c r="N6" s="41">
         <v>44162</v>
       </c>
-      <c r="O6" s="44">
+      <c r="O6" s="41">
         <v>44169</v>
       </c>
-      <c r="P6" s="44">
+      <c r="P6" s="41">
         <v>44176</v>
       </c>
-      <c r="Q6" s="44">
+      <c r="Q6" s="41">
         <v>44183</v>
       </c>
-      <c r="R6" s="44">
+      <c r="R6" s="41">
         <v>44190</v>
       </c>
-      <c r="S6" s="44">
+      <c r="S6" s="41">
         <v>44197</v>
       </c>
-      <c r="T6" s="44">
+      <c r="T6" s="41">
         <v>44204</v>
       </c>
-      <c r="U6" s="44">
+      <c r="U6" s="41">
         <v>44211</v>
       </c>
-      <c r="V6" s="7">
+      <c r="V6" s="41">
         <v>44218</v>
       </c>
-      <c r="W6" s="7">
+      <c r="W6" s="6">
         <v>44225</v>
       </c>
-      <c r="X6" s="21">
+      <c r="X6" s="19">
         <v>44232</v>
       </c>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
+      <c r="Y6" s="19">
+        <v>44239</v>
+      </c>
+      <c r="Z6" s="47">
+        <v>44246</v>
+      </c>
+      <c r="AA6" s="47">
+        <v>44253</v>
+      </c>
     </row>
-    <row r="7" spans="1:26" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+    <row r="7" spans="1:27" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33" t="s">
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="34"/>
-      <c r="R7" s="34"/>
-      <c r="S7" s="34"/>
-      <c r="T7" s="34"/>
-      <c r="U7" s="34"/>
-      <c r="V7" s="36" t="s">
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="W7" s="37" t="s">
+      <c r="W7" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="X7" s="35"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="43"/>
+      <c r="Z7" s="43"/>
+      <c r="AA7" s="43"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="9" t="s">
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="9" t="s">
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="11" t="s">
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="S8" s="11" t="s">
+      <c r="S8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="T8" s="11" t="s">
+      <c r="T8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="U8" s="10" t="s">
+      <c r="U8" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="24" t="s">
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="44" t="s">
         <v>43</v>
       </c>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="48"/>
+      <c r="AA8" s="48"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="31" t="s">
+      <c r="E9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="31" t="s">
+      <c r="I9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="31" t="s">
+      <c r="J9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="K9" s="31" t="s">
+      <c r="K9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="M9" s="31" t="s">
+      <c r="M9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="31" t="s">
+      <c r="N9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="O9" s="31" t="s">
+      <c r="O9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="P9" s="31" t="s">
+      <c r="P9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="Q9" s="31" t="s">
+      <c r="Q9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="R9" s="31" t="s">
+      <c r="R9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="S9" s="31" t="s">
+      <c r="S9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="T9" s="31" t="s">
+      <c r="T9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="U9" s="31" t="s">
+      <c r="U9" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="V9" s="12" t="s">
+      <c r="V9" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="W9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="W9" s="13" t="s">
+      <c r="X9" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="X9" s="25" t="s">
+      <c r="Y9" s="22" t="s">
         <v>41</v>
       </c>
+      <c r="Z9" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA9" s="22" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="29" t="s">
+      <c r="E10" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="29" t="s">
+      <c r="I10" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="29" t="s">
+      <c r="J10" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="29" t="s">
+      <c r="K10" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="29" t="s">
+      <c r="L10" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="M10" s="29" t="s">
+      <c r="M10" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="29" t="s">
+      <c r="N10" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="29" t="s">
+      <c r="O10" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="P10" s="29" t="s">
+      <c r="P10" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="Q10" s="29" t="s">
+      <c r="Q10" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="R10" s="29" t="s">
+      <c r="R10" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="S10" s="29" t="s">
+      <c r="S10" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="T10" s="29" t="s">
+      <c r="T10" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="U10" s="29" t="s">
+      <c r="U10" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="V10" s="29" t="s">
+      <c r="V10" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="W10" s="29" t="s">
+      <c r="W10" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="X10" s="29" t="s">
+      <c r="X10" s="26" t="s">
         <v>39</v>
       </c>
+      <c r="Y10" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z10" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA10" s="26" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A12" s="35" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="39" t="s">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A14" s="38" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1771,18 +1866,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2009,18 +2104,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07E1F462-3555-42C8-855E-56779F9BD1EF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C82C6B7-F5A9-4C61-A0FE-73C6A14DE687}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C82C6B7-F5A9-4C61-A0FE-73C6A14DE687}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07E1F462-3555-42C8-855E-56779F9BD1EF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="72caab85-b177-4a5e-b33a-cb569996d4d6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="3c4e9300-2158-4f27-b7a4-0ea661d6437f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>